<commit_message>
read from excel tested
</commit_message>
<xml_diff>
--- a/testread1.xlsx
+++ b/testread1.xlsx
@@ -149,7 +149,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -160,9 +160,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1256,7 +1253,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1419,61 +1416,6 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>